<commit_message>
print number of rows before and after removing NAs at import and before and after removing duplicates in keytable
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2021.xlsx
+++ b/data-raw/FAKE_DATA_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC742F7F-F2F3-7F4D-9E30-D8961E4274C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B841F76-0E64-FA42-A2E6-D42320D0A67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-7260" windowWidth="38400" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="1060" yWindow="740" windowWidth="14180" windowHeight="18380" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>Sihlwald</t>
   </si>
   <si>
-    <t>Freud</t>
-  </si>
-  <si>
     <t>Ferdi</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>756.0000.0000.01</t>
+  </si>
+  <si>
+    <t>Freud-Fichter</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -578,10 +578,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
@@ -590,16 +590,16 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>19</v>
@@ -608,12 +608,12 @@
         <v>20</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -640,7 +640,7 @@
         <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2">
         <v>11</v>
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3">
         <v>22</v>
@@ -731,10 +731,10 @@
         <v>7560000000006</v>
       </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
       </c>
       <c r="D4" s="4">
         <v>28193</v>
@@ -752,10 +752,10 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4">
         <v>300</v>
@@ -764,7 +764,7 @@
         <v>852502</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4" s="5">
         <v>9</v>

</xml_diff>